<commit_message>
IMP: cambios para obtener la autorizacion de la retencion en la factura de proveedor
</commit_message>
<xml_diff>
--- a/l10n_ec_niif/data/impuestos_ec.xlsx
+++ b/l10n_ec_niif/data/impuestos_ec.xlsx
@@ -5,13 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="taxes" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="tax_support" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">taxes!$A$1:$J$95</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="679">
   <si>
     <t xml:space="preserve">tag</t>
   </si>
@@ -1050,760 +1053,1254 @@
     <t xml:space="preserve">refund_repartition_line_ids</t>
   </si>
   <si>
+    <t xml:space="preserve">tax_411_iva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_ec_niif.ec_chart_template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventas locales (excluye activos fijos) gravadas tarifa diferente de cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 12%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_ec_niif.tax_group_iva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_411')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070101'),'tag_ids': [ref('tag_f104_421')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_412_iva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventas de activos fijos gravadas tarifa diferente de cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA AF 12%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_412')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070102'),'tag_ids': [ref('tag_f104_422')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_423</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_423')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_413')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_424</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_424')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_414')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_413</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 0% SCT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_414</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA AF 0% SCT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_415</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_415')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_416</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA AF 0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_416')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_417</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA EB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_417')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_418</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_418')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_441</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Exento IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_441')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_444</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresos por reembolso como intermediario / valores facturados por operadoras de transporte (informativo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por Reembolso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_444')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070105'),'tag_ids': [ref('tag_f104_454')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_510</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Adquisiciones y pagos (excluye activos fijos) gravados tarifa diferente de cero (con derecho a crédito tributario)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_510')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050101'),'tag_ids': [ref('tag_f104_520')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_511</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Adquisiciones locales de activos fijos gravados tarifa diferente de cero (con derecho a crédito tributario) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_511')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050102'),'tag_ids': [ref('tag_f104_521')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_512</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras adquisiciones y pagos gravados tarifa diferente de cero (sin derecho a crédito tributario)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 12% SCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_512')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050103'),'tag_ids': [ref('tag_f104_522')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_513</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Importaciones de servicios y/o derechos gravados tarifa diferente de cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 12% IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_513')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050104'),'tag_ids': [ref('tag_f104_523')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_514</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Importaciones de bienes (excluye activos fijos) gravados tarifa diferente de cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 12% IB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_514')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050105'),'tag_ids': [ref('tag_f104_524')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_515</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Importaciones de activos fijos gravados tarifa diferente de cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 12% AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_515')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050106'),'tag_ids': [ref('tag_f104_525')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_526</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_526')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_527</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_527')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_516</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IVA 0% IB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_516')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_517</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_517')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_518</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">RISE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_518')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_541</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">No Objeto IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_541')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_542</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_542')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_545</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagos netos por reembolso como intermediario / valores facturados por socios a operadoras de transporte (informativo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_545')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_721_iva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 10% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_ec_niif.tax_group_iva_withhold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -10,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_721')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_723</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 20%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 20% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -20,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_723')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_725</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 30%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 30% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -30,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_725')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_727</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 50% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -50,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_727')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_729</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 70%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 70% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -70,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_729')]}),]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tax_731</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">_iva</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Retención IVA del 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ret. 100% IVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -100,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_731')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En relación de dependencia que supera o no la base desgravada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l10n_ec_niif.tax_group_renta_withhold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_303')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_353')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Honorarios profesionales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Predomina el intelecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_304')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_354')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Predomina la mano de obra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_307')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_357')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Utilización o aprovechamiento de la imagen o renombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_308')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_358')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Publicidad y comunicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_309')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_359')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servicios Transporte privado de pasajeros o servicio público o privado de carga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_310')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_360')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A través de liquidaciones de compra (nivel cultural o rusticidad)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_311')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_361')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferencia de bienes muebles de naturaleza corporal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_312')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_362')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por regalías, derechos de autor, marcas, patentes y similares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_314')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_364')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_319</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrendamiento Mercantil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_319')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_369')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arrendamiento Bienes inmuebles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_320')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_370')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguros y reaseguros (primas y cesiones)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_322')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_372')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendimientos financieros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_323')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_373')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendimientos financieros entre instituciones del sistema financiero y entidades economía popular y solidaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_324')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_374')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anticipo dividendos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_325')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_375')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos distribuidos que correspondan al impuesto a la renta único establecido en el art. 27 de la LRTI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_326')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos distribuidos a personas naturales residentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_327')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos distribuidos a sociedades residentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_328')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_329</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos distribuidos a fideicomisos residentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_329')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos gravados distribuidos en acciones (reinversión de utilidades sin derecho a reducción tarifa IR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_330')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendos exentos distribuidos en acciones (reinversión de utilidades con derecho a reducción tarifa IR) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_331')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagos de bienes y servicios no sujetos a retención</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_332')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enajenación de derechos representativos de capital y otros derechos cotizados en bolsa ecuatoriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_333')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_383')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enajenación de derechos representativos de capital y otros derechos no cotizados en bolsa ecuatoriana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_334')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_384')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loterías, rifas, apuestas y similares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_335')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_385')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_343</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicables el 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_343')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_393')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_344</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicables el 2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_344')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_394')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicables el 8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_345')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_395')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicables a otros porcentajes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_346')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_402')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_452')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Intereses de créditos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_403')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_453')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Anticipo de dividendos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_404')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_454')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a personas naturales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_405')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a sociedades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_406')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_456')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a fideicomisos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_407')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_457')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Enajenación de derechos representativos de capital y otros derechos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_408')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_458')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Seguros y reaseguros (primas y cesiones)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_409')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_459')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con convenio de doble tributación Servicios técnicos, administrativos o de consultoría y regalías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_410')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_460')]}),]</t>
+  </si>
+  <si>
     <t xml:space="preserve">tax_411</t>
   </si>
   <si>
-    <t xml:space="preserve">l10n_ec_niif.ec_chart_template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ventas locales (excluye activos fijos) gravadas tarifa diferente de cero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 12%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_ec_niif.tax_group_iva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_411')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070101'),'tag_ids': [ref('tag_f104_421')]}),]</t>
+    <t xml:space="preserve">Con convenio de doble tributación Otros conceptos de ingresos gravados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_411')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_461')]}),]</t>
   </si>
   <si>
     <t xml:space="preserve">tax_412</t>
   </si>
   <si>
-    <t xml:space="preserve">Ventas de activos fijos gravadas tarifa diferente de cero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA AF 12%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_412')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070102'),'tag_ids': [ref('tag_f104_422')]}),]</t>
+    <t xml:space="preserve">Con convenio de doble tributación Otros pagos al exterior no sujetos a retención</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_412')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Intereses por financiamiento de proveedores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Intereses de créditos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Anticipo de dividendos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a personas naturales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_416')]}),] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_417</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a sociedades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_417')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_467')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_418</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a fideicomisos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_418')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_468')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Enajenación de derechos representativos de capital y otros derechos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_419')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_469')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Seguros y reaseguros (primas y cesiones)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_420')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_470')]}),]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Servicios técnicos, administrativos o de consultoría y regalías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax_422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin convenio de doble tributación Otros conceptos de ingresos gravados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_422')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_472')]}),]</t>
   </si>
   <si>
     <t xml:space="preserve">tax_423</t>
   </si>
   <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_423')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_413')]}),]</t>
+    <t xml:space="preserve">Sin convenio de doble tributación Otros pagos al exterior no sujetos a retención</t>
   </si>
   <si>
     <t xml:space="preserve">tax_424</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_424')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_414')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_413</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 0% SCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_414</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA AF 0% SCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_415</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_415')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA AF 0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_416')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA EB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_417')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_418</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_418')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exento IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_441')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_444</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresos por reembolso como intermediario / valores facturados por operadoras de transporte (informativo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por Reembolso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_444')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('201070105'),'tag_ids': [ref('tag_f104_454')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_510</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adquisiciones y pagos (excluye activos fijos) gravados tarifa diferente de cero (con derecho a crédito tributario)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_510')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050101'),'tag_ids': [ref('tag_f104_520')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adquisiciones locales de activos fijos gravados tarifa diferente de cero (con derecho a crédito tributario) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_511')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050102'),'tag_ids': [ref('tag_f104_521')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_512</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras adquisiciones y pagos gravados tarifa diferente de cero (sin derecho a crédito tributario)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 12% SCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_512')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050103'),'tag_ids': [ref('tag_f104_522')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importaciones de servicios y/o derechos gravados tarifa diferente de cero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 12% IS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_513')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050104'),'tag_ids': [ref('tag_f104_523')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importaciones de bienes (excluye activos fijos) gravados tarifa diferente de cero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 12% IB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_514')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050105'),'tag_ids': [ref('tag_f104_524')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_515</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importaciones de activos fijos gravados tarifa diferente de cero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 12% AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_515')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050106'),'tag_ids': [ref('tag_f104_525')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_526</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_526')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_527</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_527')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVA 0% IB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_516')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_517')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_518</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RISE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_518')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Objeto IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_541')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_542</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_542')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_545</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagos netos por reembolso como intermediario / valores facturados por socios a operadoras de transporte (informativo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f104_545')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_721</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 10%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 10% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_ec_niif.tax_group_iva_withhold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -10,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_721')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_723</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 20%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 20% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -20,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_723')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_725</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 30%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 30% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -30,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_725')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 50% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -50,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_727')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_729</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 70%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 70% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -70,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_729')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retención IVA del 100%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ret. 100% IVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': []}), (0,0, {'factor_percent': -100,'repartition_type': 'tax','account_id': ref('101050107'),'tag_ids': [ref('tag_f104_731')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En relación de dependencia que supera o no la base desgravada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">l10n_ec_niif.tax_group_renta_withhold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_303')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_353')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_303</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Honorarios profesionales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Predomina el intelecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_304')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_354')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Predomina la mano de obra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_307')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_357')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Utilización o aprovechamiento de la imagen o renombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_308')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_358')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Publicidad y comunicación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_309')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_359')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_310</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servicios Transporte privado de pasajeros o servicio público o privado de carga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_310')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_360')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_311</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A través de liquidaciones de compra (nivel cultural o rusticidad)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_311')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_361')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transferencia de bienes muebles de naturaleza corporal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_312')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_362')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_314</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por regalías, derechos de autor, marcas, patentes y similares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_314')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_364')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_319</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrendamiento Mercantil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_319')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_369')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arrendamiento Bienes inmuebles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_320')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_370')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seguros y reaseguros (primas y cesiones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_322')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_372')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendimientos financieros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_323')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_373')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_324</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendimientos financieros entre instituciones del sistema financiero y entidades economía popular y solidaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_324')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_374')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_325</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anticipo dividendos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_325')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_375')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos distribuidos que correspondan al impuesto a la renta único establecido en el art. 27 de la LRTI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_326')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos distribuidos a personas naturales residentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_327')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos distribuidos a sociedades residentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_328')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_329</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos distribuidos a fideicomisos residentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_329')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos gravados distribuidos en acciones (reinversión de utilidades sin derecho a reducción tarifa IR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_330')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dividendos exentos distribuidos en acciones (reinversión de utilidades con derecho a reducción tarifa IR) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_331')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_332</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagos de bienes y servicios no sujetos a retención</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_332')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enajenación de derechos representativos de capital y otros derechos cotizados en bolsa ecuatoriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_333')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_383')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_334</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enajenación de derechos representativos de capital y otros derechos no cotizados en bolsa ecuatoriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_334')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_384')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_335</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loterías, rifas, apuestas y similares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_335')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_385')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_343</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicables el 1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_343')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_393')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_344</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicables el 2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_344')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_394')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicables el 8%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_345')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_395')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicables a otros porcentajes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_346')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_402')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_452')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_403</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Intereses de créditos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_403')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_453')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Anticipo de dividendos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_404')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_454')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a personas naturales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_405')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a sociedades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_406')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_456')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_407</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Dividendos distribuidos a fideicomisos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_407')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_457')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_408</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Enajenación de derechos representativos de capital y otros derechos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_408')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_458')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_409</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Seguros y reaseguros (primas y cesiones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_409')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_459')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Servicios técnicos, administrativos o de consultoría y regalías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_410')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_460')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Otros conceptos de ingresos gravados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_411')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_461')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con convenio de doble tributación Otros pagos al exterior no sujetos a retención</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_412')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Intereses por financiamiento de proveedores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Intereses de créditos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Anticipo de dividendos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a personas naturales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_416')]}),] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a sociedades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_417')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_467')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Dividendos distribuidos a fideicomisos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_418')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_468')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_419</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Enajenación de derechos representativos de capital y otros derechos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_419')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_469')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_420</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Seguros y reaseguros (primas y cesiones)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_420')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_470')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Servicios técnicos, administrativos o de consultoría y regalías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax_422</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Otros conceptos de ingresos gravados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[(5, 0, 0), (0,0, {'factor_percent': 100, 'repartition_type': 'base','tag_ids': [ref('tag_f103_422')]}), (0,0, {'factor_percent': 100,'repartition_type': 'tax','account_id': ref('101050201'),'tag_ids': [ref('tag_f103_472')]}),]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin convenio de doble tributación Otros pagos al exterior no sujetos a retención</t>
   </si>
   <si>
     <t xml:space="preserve">En paraísos fiscales o regímenes fiscales preferentes Intereses por financiamiento de proveedores</t>
@@ -2038,7 +2535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2142,10 +2639,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2294,7 +2797,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2316,11 +2819,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2413,6 +2916,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2424,7 +2931,7 @@
       <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="120.09"/>
@@ -6017,51 +6524,51 @@
   </sheetPr>
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="39.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="68.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="55.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>341</v>
       </c>
     </row>
@@ -6129,7 +6636,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>354</v>
       </c>
@@ -6158,7 +6665,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>357</v>
       </c>
@@ -6187,7 +6694,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>360</v>
       </c>
@@ -6219,7 +6726,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>362</v>
       </c>
@@ -6251,7 +6758,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>364</v>
       </c>
@@ -6283,7 +6790,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>367</v>
       </c>
@@ -6315,7 +6822,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>370</v>
       </c>
@@ -6347,7 +6854,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>373</v>
       </c>
@@ -6379,7 +6886,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>376</v>
       </c>
@@ -6411,7 +6918,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>379</v>
       </c>
@@ -6443,7 +6950,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>383</v>
       </c>
@@ -6475,7 +6982,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>387</v>
       </c>
@@ -6507,7 +7014,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>390</v>
       </c>
@@ -6539,7 +7046,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>394</v>
       </c>
@@ -6571,7 +7078,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>398</v>
       </c>
@@ -6603,7 +7110,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="49.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>402</v>
       </c>
@@ -6635,7 +7142,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>406</v>
       </c>
@@ -6664,7 +7171,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>408</v>
       </c>
@@ -6693,7 +7200,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>410</v>
       </c>
@@ -6725,7 +7232,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>413</v>
       </c>
@@ -6757,7 +7264,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>415</v>
       </c>
@@ -6789,7 +7296,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>418</v>
       </c>
@@ -6821,7 +7328,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>421</v>
       </c>
@@ -6853,7 +7360,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>423</v>
       </c>
@@ -6917,7 +7424,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>431</v>
       </c>
@@ -6949,7 +7456,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>435</v>
       </c>
@@ -6981,7 +7488,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>439</v>
       </c>
@@ -7013,7 +7520,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>443</v>
       </c>
@@ -7045,7 +7552,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>447</v>
       </c>
@@ -7087,6 +7594,9 @@
       <c r="C34" s="2" t="s">
         <v>452</v>
       </c>
+      <c r="D34" s="0" t="n">
+        <v>302</v>
+      </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
       </c>
@@ -7116,6 +7626,9 @@
       <c r="C35" s="2" t="s">
         <v>457</v>
       </c>
+      <c r="D35" s="0" t="n">
+        <v>303</v>
+      </c>
       <c r="E35" s="0" t="n">
         <v>-10</v>
       </c>
@@ -7145,6 +7658,9 @@
       <c r="C36" s="2" t="s">
         <v>459</v>
       </c>
+      <c r="D36" s="0" t="n">
+        <v>304</v>
+      </c>
       <c r="E36" s="0" t="n">
         <v>-8</v>
       </c>
@@ -7174,6 +7690,9 @@
       <c r="C37" s="2" t="s">
         <v>462</v>
       </c>
+      <c r="D37" s="0" t="n">
+        <v>307</v>
+      </c>
       <c r="E37" s="0" t="n">
         <v>-2</v>
       </c>
@@ -7203,6 +7722,9 @@
       <c r="C38" s="2" t="s">
         <v>465</v>
       </c>
+      <c r="D38" s="0" t="n">
+        <v>308</v>
+      </c>
       <c r="E38" s="0" t="n">
         <v>-10</v>
       </c>
@@ -7232,6 +7754,9 @@
       <c r="C39" s="2" t="s">
         <v>468</v>
       </c>
+      <c r="D39" s="0" t="n">
+        <v>309</v>
+      </c>
       <c r="E39" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7261,6 +7786,9 @@
       <c r="C40" s="2" t="s">
         <v>471</v>
       </c>
+      <c r="D40" s="0" t="n">
+        <v>310</v>
+      </c>
       <c r="E40" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7290,6 +7818,9 @@
       <c r="C41" s="2" t="s">
         <v>474</v>
       </c>
+      <c r="D41" s="0" t="n">
+        <v>311</v>
+      </c>
       <c r="E41" s="0" t="n">
         <v>-2</v>
       </c>
@@ -7319,6 +7850,9 @@
       <c r="C42" s="2" t="s">
         <v>477</v>
       </c>
+      <c r="D42" s="0" t="n">
+        <v>312</v>
+      </c>
       <c r="E42" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7348,6 +7882,9 @@
       <c r="C43" s="2" t="s">
         <v>480</v>
       </c>
+      <c r="D43" s="0" t="n">
+        <v>314</v>
+      </c>
       <c r="E43" s="0" t="n">
         <v>-8</v>
       </c>
@@ -7377,6 +7914,9 @@
       <c r="C44" s="2" t="s">
         <v>483</v>
       </c>
+      <c r="D44" s="0" t="n">
+        <v>319</v>
+      </c>
       <c r="E44" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7406,6 +7946,9 @@
       <c r="C45" s="2" t="s">
         <v>486</v>
       </c>
+      <c r="D45" s="0" t="n">
+        <v>320</v>
+      </c>
       <c r="E45" s="0" t="n">
         <v>-8</v>
       </c>
@@ -7435,6 +7978,9 @@
       <c r="C46" s="2" t="s">
         <v>489</v>
       </c>
+      <c r="D46" s="0" t="n">
+        <v>322</v>
+      </c>
       <c r="E46" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7464,6 +8010,9 @@
       <c r="C47" s="2" t="s">
         <v>492</v>
       </c>
+      <c r="D47" s="0" t="n">
+        <v>323</v>
+      </c>
       <c r="E47" s="0" t="n">
         <v>-2</v>
       </c>
@@ -7493,6 +8042,9 @@
       <c r="C48" s="2" t="s">
         <v>495</v>
       </c>
+      <c r="D48" s="0" t="n">
+        <v>324</v>
+      </c>
       <c r="E48" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7522,6 +8074,9 @@
       <c r="C49" s="2" t="s">
         <v>498</v>
       </c>
+      <c r="D49" s="0" t="n">
+        <v>325</v>
+      </c>
       <c r="E49" s="0" t="n">
         <v>-25</v>
       </c>
@@ -7551,6 +8106,9 @@
       <c r="C50" s="2" t="s">
         <v>501</v>
       </c>
+      <c r="D50" s="0" t="n">
+        <v>326</v>
+      </c>
       <c r="E50" s="0" t="n">
         <v>0</v>
       </c>
@@ -7580,6 +8138,9 @@
       <c r="C51" s="2" t="s">
         <v>504</v>
       </c>
+      <c r="D51" s="0" t="n">
+        <v>327</v>
+      </c>
       <c r="E51" s="0" t="n">
         <v>0</v>
       </c>
@@ -7609,6 +8170,9 @@
       <c r="C52" s="2" t="s">
         <v>507</v>
       </c>
+      <c r="D52" s="0" t="n">
+        <v>328</v>
+      </c>
       <c r="E52" s="0" t="n">
         <v>0</v>
       </c>
@@ -7638,6 +8202,9 @@
       <c r="C53" s="2" t="s">
         <v>510</v>
       </c>
+      <c r="D53" s="0" t="n">
+        <v>329</v>
+      </c>
       <c r="E53" s="0" t="n">
         <v>0</v>
       </c>
@@ -7667,6 +8234,9 @@
       <c r="C54" s="2" t="s">
         <v>513</v>
       </c>
+      <c r="D54" s="0" t="n">
+        <v>330</v>
+      </c>
       <c r="E54" s="0" t="n">
         <v>0</v>
       </c>
@@ -7696,6 +8266,9 @@
       <c r="C55" s="2" t="s">
         <v>516</v>
       </c>
+      <c r="D55" s="0" t="n">
+        <v>331</v>
+      </c>
       <c r="E55" s="0" t="n">
         <v>0</v>
       </c>
@@ -7725,6 +8298,9 @@
       <c r="C56" s="2" t="s">
         <v>519</v>
       </c>
+      <c r="D56" s="0" t="n">
+        <v>332</v>
+      </c>
       <c r="E56" s="0" t="n">
         <v>0</v>
       </c>
@@ -7754,6 +8330,9 @@
       <c r="C57" s="2" t="s">
         <v>522</v>
       </c>
+      <c r="D57" s="0" t="n">
+        <v>333</v>
+      </c>
       <c r="E57" s="0" t="n">
         <v>-10</v>
       </c>
@@ -7783,6 +8362,9 @@
       <c r="C58" s="2" t="s">
         <v>525</v>
       </c>
+      <c r="D58" s="0" t="n">
+        <v>334</v>
+      </c>
       <c r="E58" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7812,6 +8394,9 @@
       <c r="C59" s="2" t="s">
         <v>528</v>
       </c>
+      <c r="D59" s="0" t="n">
+        <v>335</v>
+      </c>
       <c r="E59" s="0" t="n">
         <v>-15</v>
       </c>
@@ -7841,6 +8426,9 @@
       <c r="C60" s="2" t="s">
         <v>531</v>
       </c>
+      <c r="D60" s="0" t="n">
+        <v>343</v>
+      </c>
       <c r="E60" s="0" t="n">
         <v>-1</v>
       </c>
@@ -7870,6 +8458,9 @@
       <c r="C61" s="2" t="s">
         <v>534</v>
       </c>
+      <c r="D61" s="0" t="n">
+        <v>344</v>
+      </c>
       <c r="E61" s="0" t="n">
         <v>-2</v>
       </c>
@@ -7899,6 +8490,9 @@
       <c r="C62" s="2" t="s">
         <v>537</v>
       </c>
+      <c r="D62" s="0" t="n">
+        <v>345</v>
+      </c>
       <c r="E62" s="0" t="n">
         <v>-8</v>
       </c>
@@ -7928,6 +8522,9 @@
       <c r="C63" s="2" t="s">
         <v>540</v>
       </c>
+      <c r="D63" s="0" t="n">
+        <v>346</v>
+      </c>
       <c r="E63" s="0" t="n">
         <v>0</v>
       </c>
@@ -7957,6 +8554,9 @@
       <c r="C64" s="2" t="s">
         <v>543</v>
       </c>
+      <c r="D64" s="0" t="n">
+        <v>402</v>
+      </c>
       <c r="E64" s="0" t="n">
         <v>0</v>
       </c>
@@ -7986,6 +8586,9 @@
       <c r="C65" s="2" t="s">
         <v>546</v>
       </c>
+      <c r="D65" s="0" t="n">
+        <v>403</v>
+      </c>
       <c r="E65" s="0" t="n">
         <v>0</v>
       </c>
@@ -8015,6 +8618,9 @@
       <c r="C66" s="2" t="s">
         <v>549</v>
       </c>
+      <c r="D66" s="0" t="n">
+        <v>404</v>
+      </c>
       <c r="E66" s="0" t="n">
         <v>0</v>
       </c>
@@ -8044,6 +8650,9 @@
       <c r="C67" s="2" t="s">
         <v>552</v>
       </c>
+      <c r="D67" s="0" t="n">
+        <v>405</v>
+      </c>
       <c r="E67" s="0" t="n">
         <v>0</v>
       </c>
@@ -8073,6 +8682,9 @@
       <c r="C68" s="2" t="s">
         <v>555</v>
       </c>
+      <c r="D68" s="0" t="n">
+        <v>406</v>
+      </c>
       <c r="E68" s="0" t="n">
         <v>0</v>
       </c>
@@ -8102,6 +8714,9 @@
       <c r="C69" s="2" t="s">
         <v>558</v>
       </c>
+      <c r="D69" s="0" t="n">
+        <v>407</v>
+      </c>
       <c r="E69" s="0" t="n">
         <v>0</v>
       </c>
@@ -8131,6 +8746,9 @@
       <c r="C70" s="2" t="s">
         <v>561</v>
       </c>
+      <c r="D70" s="0" t="n">
+        <v>408</v>
+      </c>
       <c r="E70" s="0" t="n">
         <v>0</v>
       </c>
@@ -8160,6 +8778,9 @@
       <c r="C71" s="2" t="s">
         <v>564</v>
       </c>
+      <c r="D71" s="0" t="n">
+        <v>409</v>
+      </c>
       <c r="E71" s="0" t="n">
         <v>0</v>
       </c>
@@ -8189,6 +8810,9 @@
       <c r="C72" s="2" t="s">
         <v>567</v>
       </c>
+      <c r="D72" s="0" t="n">
+        <v>410</v>
+      </c>
       <c r="E72" s="0" t="n">
         <v>0</v>
       </c>
@@ -8210,13 +8834,16 @@
     </row>
     <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>342</v>
+        <v>569</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>411</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>0</v>
@@ -8231,21 +8858,24 @@
         <v>454</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>350</v>
+        <v>572</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>571</v>
+        <v>573</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>412</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>0</v>
@@ -8260,21 +8890,24 @@
         <v>454</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>360</v>
+        <v>575</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>573</v>
+        <v>576</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>413</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>0</v>
@@ -8289,21 +8922,24 @@
         <v>454</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>362</v>
+        <v>577</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>574</v>
+        <v>578</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>414</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>0</v>
@@ -8318,21 +8954,24 @@
         <v>454</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>364</v>
+        <v>579</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>575</v>
+        <v>580</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>415</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>0</v>
@@ -8347,21 +8986,24 @@
         <v>454</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>367</v>
+        <v>581</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>576</v>
+        <v>582</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>416</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>0</v>
@@ -8376,21 +9018,24 @@
         <v>454</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>370</v>
+        <v>584</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>578</v>
+        <v>585</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>417</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>0</v>
@@ -8405,21 +9050,24 @@
         <v>454</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>373</v>
+        <v>587</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>580</v>
+        <v>588</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>418</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>0</v>
@@ -8434,21 +9082,24 @@
         <v>454</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>583</v>
+        <v>591</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>419</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>0</v>
@@ -8463,21 +9114,24 @@
         <v>454</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>586</v>
+        <v>594</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>420</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>0</v>
@@ -8492,21 +9146,24 @@
         <v>454</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>589</v>
+        <v>597</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>421</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>0</v>
@@ -8521,21 +9178,24 @@
         <v>454</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>591</v>
+        <v>599</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>422</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>0</v>
@@ -8550,21 +9210,24 @@
         <v>454</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>354</v>
+        <v>601</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>593</v>
+        <v>602</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>423</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>0</v>
@@ -8587,13 +9250,16 @@
     </row>
     <row r="86" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>357</v>
+        <v>603</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>594</v>
+        <v>604</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>424</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>0</v>
@@ -8608,21 +9274,24 @@
         <v>454</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>597</v>
+        <v>607</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>425</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>0</v>
@@ -8637,21 +9306,24 @@
         <v>454</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>600</v>
+        <v>610</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>426</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>0</v>
@@ -8666,21 +9338,24 @@
         <v>454</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>603</v>
+        <v>613</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>427</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>0</v>
@@ -8695,21 +9370,24 @@
         <v>454</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>606</v>
+        <v>616</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>428</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>0</v>
@@ -8724,21 +9402,24 @@
         <v>454</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>608</v>
+        <v>618</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>609</v>
+        <v>619</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>429</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>0</v>
@@ -8753,21 +9434,24 @@
         <v>454</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>612</v>
+        <v>622</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>430</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>0</v>
@@ -8782,21 +9466,24 @@
         <v>454</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>615</v>
+        <v>625</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>431</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>0</v>
@@ -8811,21 +9498,24 @@
         <v>454</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>618</v>
+        <v>628</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>432</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>0</v>
@@ -8840,21 +9530,24 @@
         <v>454</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>343</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>621</v>
+        <v>631</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>433</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>0</v>
@@ -8869,20 +9562,22 @@
         <v>454</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>622</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J95"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8893,11 +9588,11 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="49.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="53.63"/>
@@ -8908,13 +9603,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>623</v>
+        <v>633</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>624</v>
+        <v>634</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8923,13 +9618,13 @@
         <v>ts_01</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>625</v>
+        <v>635</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>626</v>
+        <v>636</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>627</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8938,13 +9633,13 @@
         <v>ts_02</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>629</v>
+        <v>639</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>630</v>
+        <v>640</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8953,13 +9648,13 @@
         <v>ts_03</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>631</v>
+        <v>641</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>632</v>
+        <v>642</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>633</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8968,13 +9663,13 @@
         <v>ts_04</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>634</v>
+        <v>644</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>636</v>
+        <v>646</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8983,13 +9678,13 @@
         <v>ts_05</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>638</v>
+        <v>648</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>639</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="47.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8998,13 +9693,13 @@
         <v>ts_06</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>641</v>
+        <v>651</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>642</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9013,13 +9708,13 @@
         <v>ts_07</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>643</v>
+        <v>653</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>644</v>
+        <v>654</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>645</v>
+        <v>655</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9028,13 +9723,13 @@
         <v>ts_08</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>646</v>
+        <v>656</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>647</v>
+        <v>657</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>648</v>
+        <v>658</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9043,13 +9738,13 @@
         <v>ts_09</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9058,13 +9753,13 @@
         <v>ts_10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>652</v>
+        <v>662</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>653</v>
+        <v>663</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9073,13 +9768,13 @@
         <v>ts_11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>655</v>
+        <v>665</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>656</v>
+        <v>666</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>657</v>
+        <v>667</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9088,13 +9783,13 @@
         <v>ts_12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>658</v>
+        <v>668</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>659</v>
+        <v>669</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>660</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9103,13 +9798,13 @@
         <v>ts_13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>662</v>
+        <v>672</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>654</v>
+        <v>664</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9118,13 +9813,13 @@
         <v>ts_14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>663</v>
+        <v>673</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>664</v>
+        <v>674</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>665</v>
+        <v>675</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9133,13 +9828,13 @@
         <v>ts_00</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>667</v>
+        <v>677</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>668</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -9147,8 +9842,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>